<commit_message>
Add dummy long name to see consequences to format
</commit_message>
<xml_diff>
--- a/01_tableOfDrivers.xlsx
+++ b/01_tableOfDrivers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t xml:space="preserve">driver</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t xml:space="preserve">ErnieTown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ErnieAliasBertiBertLongNameTest</t>
   </si>
 </sst>
 </file>
@@ -74,7 +77,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -102,6 +105,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -146,7 +154,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -155,14 +163,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -172,17 +184,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="11.35546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -254,10 +264,36 @@
         <v>14</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>24685</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Extend testing data: ßä in Streetname; non-round numbers
</commit_message>
<xml_diff>
--- a/01_tableOfDrivers.xlsx
+++ b/01_tableOfDrivers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t xml:space="preserve">driver</t>
   </si>
@@ -68,6 +68,18 @@
   </si>
   <si>
     <t xml:space="preserve">ErnieAliasBertiBertLongNameTest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sträßchen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oberbärenbad</t>
   </si>
 </sst>
 </file>
@@ -77,7 +89,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -105,11 +117,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -163,18 +170,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -184,15 +191,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.35546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="11.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -287,8 +296,28 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>76253</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>